<commit_message>
fix: added unit test and example for improved domain match
</commit_message>
<xml_diff>
--- a/test/spec_example.xlsx
+++ b/test/spec_example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottwilson/PycharmProjects/mario/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024606A1-7E02-F94B-89C4-C1C80624585B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5411F9A-9DE4-6445-922B-095FD268B99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1240" yWindow="2480" windowWidth="27640" windowHeight="11740" xr2:uid="{0338058F-5AA6-B54B-A986-17979915A6EA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
   <si>
     <t>UniqueID</t>
   </si>
@@ -183,6 +183,15 @@
   </si>
   <si>
     <t>(First Class / Same Day / Second Class/Standard Class)</t>
+  </si>
+  <si>
+    <t>Nationality (UK/ EU/ Non-EU/ Unknown) (2022/23 onwards)</t>
+  </si>
+  <si>
+    <t>Nationality</t>
+  </si>
+  <si>
+    <t>(UK/ EU/ Non-EU/ Unknown)</t>
   </si>
 </sst>
 </file>
@@ -366,7 +375,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -970,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4575CC8-0E0D-3A4D-A97B-8E154D08BAA9}">
   <dimension ref="A1:AM1100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1539,27 +1548,91 @@
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
+      <c r="A8">
+        <v>100006</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" t="s">
+        <v>50</v>
+      </c>
       <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
-      <c r="J8"/>
-      <c r="K8"/>
-      <c r="L8"/>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8" t="s">
+        <v>38</v>
+      </c>
       <c r="M8"/>
       <c r="N8"/>
       <c r="O8"/>
       <c r="P8"/>
-      <c r="Q8"/>
+      <c r="Q8" t="s">
+        <v>50</v>
+      </c>
       <c r="R8"/>
       <c r="S8"/>
       <c r="T8"/>
-      <c r="U8"/>
-      <c r="Y8"/>
-      <c r="Z8"/>
+      <c r="U8" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="V8" t="str">
+        <f>DataItems[[#This Row],[Collection]]&amp;DataItems[[#This Row],[Field]]&amp;DataItems[[#This Row],[Options for supplying the Field]]&amp;DataItems[[#This Row],[Fieldname]]&amp;DataItems[[#This Row],[Parent]]</f>
+        <v>SupserstoreNationality(UK/ EU/ Non-EU/ Unknown)Nationality</v>
+      </c>
+      <c r="W8" s="3">
+        <v>44854</v>
+      </c>
+      <c r="X8" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y8" s="4" t="str">
+        <f t="shared" ref="Y8" si="6">IF(O8="","",O8)</f>
+        <v/>
+      </c>
+      <c r="Z8" s="4" t="str">
+        <f>IF(Q8="","",IF(IFERROR(SEARCH("select",Q8)&gt;0,0),IF(S8="",IF(MID(Q8,SEARCH(F8,Q8)-4,1)=" ",MID(Q8,SEARCH(F8,Q8)-2,LEN(M25)+2),MID(Q8,SEARCH(F8,Q8)-3,LEN(F8)+3)),S8&amp;"."&amp;F8),Q8))</f>
+        <v>Nationality</v>
+      </c>
+      <c r="AA8" s="4" t="str">
+        <f t="shared" ref="AA8" si="7">IF(P8="","",P8)</f>
+        <v/>
+      </c>
+      <c r="AB8" s="4" t="str">
+        <f t="shared" ref="AB8" si="8">IF(R8="","",IF(IFERROR(SEARCH("select",R8)&gt;0,0),IF(S8="",IF(MID(R8,SEARCH(F8,R8)-4,1)=" ",MID(R8,SEARCH(F8,R8)-2,LEN(M19)+2),MID(R8,SEARCH(F8,R8)-3,LEN(F8)+3)),S8&amp;"."&amp;F8),R8))</f>
+        <v/>
+      </c>
+      <c r="AC8" t="str">
+        <f t="shared" ref="AC8" si="9">IF(D8="","","["&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(D8,"[","{"),"]","}"),"⁽"&amp;CHAR(185)&amp;"⁾","")&amp;"]")</f>
+        <v>[Nationality]</v>
+      </c>
+      <c r="AH8" s="4" t="str">
+        <f t="shared" ref="AH8" si="10">IF(AG8="","",IF(IFERROR(SEARCH("select",AG8)&gt;0,0),IF(S8="",IF(MID(AG8,SEARCH(F8,AG8)-4,1)=" ",MID(AG8,SEARCH(F8,AG8)-2,LEN(M7)+2),MID(AG8,SEARCH(F8,AG8)-3,LEN(F8)+3)),S8&amp;"."&amp;F8),AG8))</f>
+        <v/>
+      </c>
+      <c r="AI8" t="str">
+        <f t="shared" ref="AI8" si="11">IF(AF8="","",AF8)</f>
+        <v/>
+      </c>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.2">
       <c r="C9"/>
@@ -2838,4 +2911,10 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{ec1a080c-7386-44f3-81c6-2c71b2b3b237}" enabled="1" method="Standard" siteId="{48f9394d-8a14-4d27-82a6-f35f12361205}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>